<commit_message>
more cases in play turn
</commit_message>
<xml_diff>
--- a/Assets/story_script.xlsx
+++ b/Assets/story_script.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\BCI-GAME\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2511F3B7-4C8B-49C9-8E65-2296E8482A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3343A4-5DB2-4DD5-9724-9D905D736A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Script" sheetId="1" r:id="rId1"/>
@@ -1876,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B63" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>

</xml_diff>